<commit_message>
Implemented getting kafka relations.
</commit_message>
<xml_diff>
--- a/data/backend/activity-client_structure.xlsx
+++ b/data/backend/activity-client_structure.xlsx
@@ -511,31 +511,37 @@
     <t>long</t>
   </si>
   <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>$VALUES</t>
+  </si>
+  <si>
+    <t>HIGHEST</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
     <t>HIGH</t>
   </si>
   <si>
-    <t>HIGHEST</t>
-  </si>
-  <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
     <t>LOWEST</t>
   </si>
   <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>$VALUES</t>
-  </si>
-  <si>
     <t>isConfirmed</t>
   </si>
   <si>
+    <t>subscriptionDate</t>
+  </si>
+  <si>
     <t>emailAddress</t>
   </si>
   <si>
-    <t>subscriptionDate</t>
+    <t>observingUsers</t>
+  </si>
+  <si>
+    <t>imageUrl</t>
   </si>
   <si>
     <t>key</t>
@@ -547,10 +553,7 @@
     <t>observedUsers</t>
   </si>
   <si>
-    <t>imageUrl</t>
-  </si>
-  <si>
-    <t>observingUsers</t>
+    <t>query</t>
   </si>
   <si>
     <t>pageSize</t>
@@ -559,70 +562,67 @@
     <t>pageNumber</t>
   </si>
   <si>
-    <t>query</t>
+    <t>street</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
     <t>phoneNumber</t>
   </si>
   <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>street</t>
-  </si>
-  <si>
-    <t>dateOfBirth</t>
-  </si>
-  <si>
-    <t>postalCode</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>profileImageUrl</t>
   </si>
   <si>
+    <t>firstName</t>
+  </si>
+  <si>
     <t>city</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>firstName</t>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>ORDER</t>
   </si>
   <si>
     <t>FORUM</t>
   </si>
   <si>
-    <t>ORDER</t>
-  </si>
-  <si>
-    <t>PRODUCT</t>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>affectedUsers</t>
+  </si>
+  <si>
+    <t>relatedId</t>
   </si>
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>affectedUsers</t>
-  </si>
-  <si>
     <t>eventTimestamp</t>
   </si>
   <si>
-    <t>relatedId</t>
-  </si>
-  <si>
     <t>acknowledgedUsers</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>domain</t>
   </si>
   <si>
     <t>Source Class Name</t>
@@ -7298,10 +7298,10 @@
         <v>164</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -7354,10 +7354,10 @@
         <v>168</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14">
@@ -7385,7 +7385,7 @@
         <v>45</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16">
@@ -7399,7 +7399,7 @@
         <v>45</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>127</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -7455,7 +7455,7 @@
         <v>45</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21">
@@ -7483,7 +7483,7 @@
         <v>45</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
@@ -7525,7 +7525,7 @@
         <v>45</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>76</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26">
@@ -7553,7 +7553,7 @@
         <v>45</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28">
@@ -7603,7 +7603,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>45</v>
@@ -7617,7 +7617,7 @@
         <v>86</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>45</v>
@@ -7785,7 +7785,7 @@
         <v>83</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C44" t="s" s="0">
         <v>45</v>
@@ -7799,13 +7799,13 @@
         <v>83</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C45" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>76</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
@@ -7813,13 +7813,13 @@
         <v>83</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47">
@@ -7883,13 +7883,13 @@
         <v>105</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52">
@@ -7897,7 +7897,7 @@
         <v>105</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C52" t="s" s="0">
         <v>6</v>
@@ -7911,13 +7911,13 @@
         <v>105</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54">
@@ -7973,7 +7973,7 @@
         <v>45</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>13</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58">
@@ -7987,7 +7987,7 @@
         <v>45</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59">
@@ -8001,7 +8001,7 @@
         <v>45</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60">
@@ -8009,7 +8009,7 @@
         <v>109</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C60" t="s" s="0">
         <v>45</v>
@@ -8023,13 +8023,13 @@
         <v>109</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C61" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62">
@@ -8037,7 +8037,7 @@
         <v>109</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="C62" t="s" s="0">
         <v>45</v>
@@ -8057,7 +8057,7 @@
         <v>45</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>42</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64">
@@ -8071,7 +8071,7 @@
         <v>45</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65">
@@ -8121,13 +8121,13 @@
         <v>111</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C68" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69">
@@ -8135,7 +8135,7 @@
         <v>111</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C69" t="s" s="0">
         <v>45</v>
@@ -8155,7 +8155,7 @@
         <v>45</v>
       </c>
       <c r="D70" t="s" s="0">
-        <v>42</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71">
@@ -8163,13 +8163,13 @@
         <v>111</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C71" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D71" t="s" s="0">
-        <v>105</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72">
@@ -8177,7 +8177,7 @@
         <v>111</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C72" t="s" s="0">
         <v>45</v>
@@ -8191,13 +8191,13 @@
         <v>111</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C73" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D73" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74">
@@ -8205,7 +8205,7 @@
         <v>111</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C74" t="s" s="0">
         <v>45</v>
@@ -8225,7 +8225,7 @@
         <v>45</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76">
@@ -8233,7 +8233,7 @@
         <v>87</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C76" t="s" s="0">
         <v>45</v>
@@ -8247,7 +8247,7 @@
         <v>87</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C77" t="s" s="0">
         <v>45</v>
@@ -8261,13 +8261,13 @@
         <v>62</v>
       </c>
       <c r="B78" t="s" s="0">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C78" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D78" t="s" s="0">
-        <v>13</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79">
@@ -8281,7 +8281,7 @@
         <v>45</v>
       </c>
       <c r="D79" t="s" s="0">
-        <v>127</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80">
@@ -8289,13 +8289,13 @@
         <v>62</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C80" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D80" t="s" s="0">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="81">
@@ -8303,7 +8303,7 @@
         <v>95</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C81" t="s" s="0">
         <v>45</v>
@@ -8317,7 +8317,7 @@
         <v>95</v>
       </c>
       <c r="B82" t="s" s="0">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C82" t="s" s="0">
         <v>45</v>
@@ -8331,7 +8331,7 @@
         <v>95</v>
       </c>
       <c r="B83" t="s" s="0">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C83" t="s" s="0">
         <v>45</v>
@@ -8387,7 +8387,7 @@
         <v>95</v>
       </c>
       <c r="B87" t="s" s="0">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C87" t="s" s="0">
         <v>45</v>
@@ -8401,7 +8401,7 @@
         <v>95</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C88" t="s" s="0">
         <v>45</v>
@@ -8415,7 +8415,7 @@
         <v>95</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C89" t="s" s="0">
         <v>45</v>
@@ -8429,7 +8429,7 @@
         <v>95</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C90" t="s" s="0">
         <v>45</v>
@@ -8443,7 +8443,7 @@
         <v>95</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C91" t="s" s="0">
         <v>45</v>
@@ -8457,13 +8457,13 @@
         <v>70</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C92" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D92" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93">
@@ -8471,13 +8471,13 @@
         <v>70</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C93" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D93" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94">
@@ -8485,7 +8485,7 @@
         <v>70</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C94" t="s" s="0">
         <v>45</v>
@@ -8499,13 +8499,13 @@
         <v>70</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C95" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D95" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="96">
@@ -8513,13 +8513,13 @@
         <v>70</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C96" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D96" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97">
@@ -8527,13 +8527,13 @@
         <v>153</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C97" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D97" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="98">
@@ -8541,13 +8541,13 @@
         <v>153</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C98" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D98" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99">

</xml_diff>

<commit_message>
Implemented getting number of lines for methods and classes.
</commit_message>
<xml_diff>
--- a/data/backend/activity-client_structure.xlsx
+++ b/data/backend/activity-client_structure.xlsx
@@ -15,12 +15,14 @@
     <sheet name="interfaceToInterfaceRelations" r:id="rId9" sheetId="7"/>
     <sheet name="fieldClassRelations" r:id="rId10" sheetId="8"/>
     <sheet name="fieldInterfaceRelations" r:id="rId11" sheetId="9"/>
+    <sheet name="classNumberOfLines" r:id="rId12" sheetId="10"/>
+    <sheet name="methodNumberOfLines" r:id="rId13" sheetId="11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2416" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2801" uniqueCount="232">
   <si>
     <t>Class Name</t>
   </si>
@@ -502,99 +504,99 @@
     <t>Field Type</t>
   </si>
   <si>
+    <t>serialVersionUID</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
     <t>$assertionsDisabled</t>
   </si>
   <si>
-    <t>serialVersionUID</t>
-  </si>
-  <si>
-    <t>long</t>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>LOWEST</t>
   </si>
   <si>
     <t>MEDIUM</t>
   </si>
   <si>
+    <t>LOW</t>
+  </si>
+  <si>
     <t>$VALUES</t>
   </si>
   <si>
     <t>HIGHEST</t>
   </si>
   <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>HIGH</t>
-  </si>
-  <si>
-    <t>LOWEST</t>
+    <t>emailAddress</t>
+  </si>
+  <si>
+    <t>subscriptionDate</t>
   </si>
   <si>
     <t>isConfirmed</t>
   </si>
   <si>
-    <t>subscriptionDate</t>
-  </si>
-  <si>
-    <t>emailAddress</t>
+    <t>key</t>
+  </si>
+  <si>
+    <t>imageUrl</t>
+  </si>
+  <si>
+    <t>observedUsers</t>
+  </si>
+  <si>
+    <t>username</t>
   </si>
   <si>
     <t>observingUsers</t>
   </si>
   <si>
-    <t>imageUrl</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>observedUsers</t>
-  </si>
-  <si>
     <t>query</t>
   </si>
   <si>
+    <t>pageNumber</t>
+  </si>
+  <si>
     <t>pageSize</t>
   </si>
   <si>
-    <t>pageNumber</t>
+    <t>city</t>
+  </si>
+  <si>
+    <t>profileImageUrl</t>
   </si>
   <si>
     <t>street</t>
   </si>
   <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
     <t>postalCode</t>
   </si>
   <si>
-    <t>gender</t>
+    <t>phoneNumber</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
-    <t>dateOfBirth</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
-    <t>profileImageUrl</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
     <t>PRODUCT</t>
   </si>
   <si>
@@ -607,24 +609,24 @@
     <t>priority</t>
   </si>
   <si>
+    <t>eventTimestamp</t>
+  </si>
+  <si>
+    <t>affectedUsers</t>
+  </si>
+  <si>
+    <t>relatedId</t>
+  </si>
+  <si>
+    <t>acknowledgedUsers</t>
+  </si>
+  <si>
     <t>domain</t>
   </si>
   <si>
-    <t>affectedUsers</t>
-  </si>
-  <si>
-    <t>relatedId</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>eventTimestamp</t>
-  </si>
-  <si>
-    <t>acknowledgedUsers</t>
-  </si>
-  <si>
     <t>Source Class Name</t>
   </si>
   <si>
@@ -662,6 +664,60 @@
   </si>
   <si>
     <t>Target Field Name</t>
+  </si>
+  <si>
+    <t>Number of Lines</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -7143,6 +7199,1459 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C113"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>97</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="C72" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>120</v>
+      </c>
+      <c r="C73" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="C74" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="C75" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="C76" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="C77" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B78" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="C78" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B79" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="C79" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B80" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C80" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B81" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="C81" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="B82" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="C82" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B83" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C83" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B84" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="C84" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B85" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="C85" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B86" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="C86" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B87" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C87" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B88" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="C88" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B89" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="C89" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B90" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C90" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B91" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C91" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B92" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="C92" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B93" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="C93" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B94" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="C94" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="C95" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="C96" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="C97" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B98" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="C98" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B99" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C99" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B100" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C100" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B101" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="C101" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B102" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="C102" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B103" t="s" s="0">
+        <v>151</v>
+      </c>
+      <c r="C103" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B104" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="C104" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B105" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="C105" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B106" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="C106" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B107" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="C107" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B108" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="C108" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B109" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="C109" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B110" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s" s="0">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B111" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="C111" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B112" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C112" t="s" s="0">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B113" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C113" t="s" s="0">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D1"/>
@@ -7203,7 +8712,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3">
@@ -7211,13 +8720,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -7225,13 +8734,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5">
@@ -7245,7 +8754,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6">
@@ -7253,13 +8762,13 @@
         <v>41</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -7267,13 +8776,13 @@
         <v>41</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8">
@@ -7298,10 +8807,10 @@
         <v>164</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -7340,10 +8849,10 @@
         <v>167</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
@@ -7371,7 +8880,7 @@
         <v>45</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>133</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -7399,7 +8908,7 @@
         <v>45</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>13</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17">
@@ -7413,7 +8922,7 @@
         <v>25</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
@@ -7421,13 +8930,13 @@
         <v>66</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
@@ -7435,13 +8944,13 @@
         <v>66</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20">
@@ -7455,7 +8964,7 @@
         <v>45</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -7483,7 +8992,7 @@
         <v>45</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23">
@@ -7567,7 +9076,7 @@
         <v>25</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29">
@@ -7575,13 +9084,13 @@
         <v>85</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
@@ -7589,13 +9098,13 @@
         <v>85</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31">
@@ -7785,7 +9294,7 @@
         <v>83</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C44" t="s" s="0">
         <v>45</v>
@@ -7799,13 +9308,13 @@
         <v>83</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C45" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46">
@@ -7813,13 +9322,13 @@
         <v>83</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>76</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47">
@@ -7833,7 +9342,7 @@
         <v>25</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48">
@@ -7841,13 +9350,13 @@
         <v>104</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C48" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
@@ -7855,13 +9364,13 @@
         <v>104</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50">
@@ -7883,13 +9392,13 @@
         <v>105</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52">
@@ -7897,13 +9406,13 @@
         <v>105</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53">
@@ -7931,7 +9440,7 @@
         <v>25</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55">
@@ -7939,13 +9448,13 @@
         <v>108</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C55" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
@@ -7953,13 +9462,13 @@
         <v>108</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C56" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57">
@@ -7987,7 +9496,7 @@
         <v>45</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59">
@@ -7995,13 +9504,13 @@
         <v>109</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C59" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60">
@@ -8009,13 +9518,13 @@
         <v>109</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C60" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61">
@@ -8043,7 +9552,7 @@
         <v>45</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63">
@@ -8057,7 +9566,7 @@
         <v>45</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64">
@@ -8071,7 +9580,7 @@
         <v>45</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65">
@@ -8085,7 +9594,7 @@
         <v>25</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66">
@@ -8093,13 +9602,13 @@
         <v>118</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C66" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -8107,13 +9616,13 @@
         <v>118</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C67" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68">
@@ -8121,13 +9630,13 @@
         <v>111</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C68" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>105</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69">
@@ -8135,13 +9644,13 @@
         <v>111</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C69" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D69" t="s" s="0">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70">
@@ -8149,13 +9658,13 @@
         <v>111</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C70" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D70" t="s" s="0">
-        <v>127</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71">
@@ -8163,13 +9672,13 @@
         <v>111</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C71" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D71" t="s" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72">
@@ -8177,13 +9686,13 @@
         <v>111</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C72" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73">
@@ -8191,7 +9700,7 @@
         <v>111</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C73" t="s" s="0">
         <v>45</v>
@@ -8205,7 +9714,7 @@
         <v>111</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="C74" t="s" s="0">
         <v>45</v>
@@ -8225,7 +9734,7 @@
         <v>45</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76">
@@ -8267,7 +9776,7 @@
         <v>45</v>
       </c>
       <c r="D78" t="s" s="0">
-        <v>133</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79">
@@ -8281,7 +9790,7 @@
         <v>45</v>
       </c>
       <c r="D79" t="s" s="0">
-        <v>13</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80">
@@ -8303,7 +9812,7 @@
         <v>95</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C81" t="s" s="0">
         <v>45</v>
@@ -8317,7 +9826,7 @@
         <v>95</v>
       </c>
       <c r="B82" t="s" s="0">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C82" t="s" s="0">
         <v>45</v>
@@ -8345,7 +9854,7 @@
         <v>95</v>
       </c>
       <c r="B84" t="s" s="0">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C84" t="s" s="0">
         <v>45</v>
@@ -8359,7 +9868,7 @@
         <v>95</v>
       </c>
       <c r="B85" t="s" s="0">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C85" t="s" s="0">
         <v>45</v>
@@ -8373,7 +9882,7 @@
         <v>95</v>
       </c>
       <c r="B86" t="s" s="0">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C86" t="s" s="0">
         <v>45</v>
@@ -8387,7 +9896,7 @@
         <v>95</v>
       </c>
       <c r="B87" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C87" t="s" s="0">
         <v>45</v>
@@ -8401,7 +9910,7 @@
         <v>95</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C88" t="s" s="0">
         <v>45</v>
@@ -8415,7 +9924,7 @@
         <v>95</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C89" t="s" s="0">
         <v>45</v>
@@ -8429,7 +9938,7 @@
         <v>95</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C90" t="s" s="0">
         <v>45</v>
@@ -8443,7 +9952,7 @@
         <v>95</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C91" t="s" s="0">
         <v>45</v>
@@ -8457,7 +9966,7 @@
         <v>70</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C92" t="s" s="0">
         <v>45</v>
@@ -8471,7 +9980,7 @@
         <v>70</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C93" t="s" s="0">
         <v>45</v>
@@ -8485,7 +9994,7 @@
         <v>70</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C94" t="s" s="0">
         <v>45</v>
@@ -8513,7 +10022,7 @@
         <v>70</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C96" t="s" s="0">
         <v>45</v>
@@ -8527,13 +10036,13 @@
         <v>153</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C97" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D97" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98">
@@ -8541,7 +10050,7 @@
         <v>153</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C98" t="s" s="0">
         <v>25</v>
@@ -8555,13 +10064,13 @@
         <v>153</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C99" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented getting standard relationship between microservices and started implementing MSM measure.
</commit_message>
<xml_diff>
--- a/data/backend/activity-client_structure.xlsx
+++ b/data/backend/activity-client_structure.xlsx
@@ -504,55 +504,58 @@
     <t>Field Type</t>
   </si>
   <si>
+    <t>$assertionsDisabled</t>
+  </si>
+  <si>
     <t>serialVersionUID</t>
   </si>
   <si>
     <t>long</t>
   </si>
   <si>
-    <t>$assertionsDisabled</t>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>LOWEST</t>
   </si>
   <si>
     <t>HIGH</t>
   </si>
   <si>
-    <t>LOWEST</t>
+    <t>HIGHEST</t>
+  </si>
+  <si>
+    <t>$VALUES</t>
   </si>
   <si>
     <t>MEDIUM</t>
   </si>
   <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>$VALUES</t>
-  </si>
-  <si>
-    <t>HIGHEST</t>
-  </si>
-  <si>
     <t>emailAddress</t>
   </si>
   <si>
+    <t>isConfirmed</t>
+  </si>
+  <si>
     <t>subscriptionDate</t>
   </si>
   <si>
-    <t>isConfirmed</t>
+    <t>observedUsers</t>
+  </si>
+  <si>
+    <t>observingUsers</t>
+  </si>
+  <si>
+    <t>imageUrl</t>
   </si>
   <si>
     <t>key</t>
   </si>
   <si>
-    <t>imageUrl</t>
-  </si>
-  <si>
-    <t>observedUsers</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
-    <t>observingUsers</t>
+    <t>pageSize</t>
   </si>
   <si>
     <t>query</t>
@@ -561,18 +564,24 @@
     <t>pageNumber</t>
   </si>
   <si>
-    <t>pageSize</t>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>profileImageUrl</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
   <si>
     <t>city</t>
   </si>
   <si>
-    <t>profileImageUrl</t>
-  </si>
-  <si>
-    <t>street</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -582,19 +591,13 @@
     <t>lastName</t>
   </si>
   <si>
-    <t>dateOfBirth</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
     <t>postalCode</t>
   </si>
   <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
-    <t>description</t>
+    <t>FORUM</t>
   </si>
   <si>
     <t>PRODUCT</t>
@@ -603,7 +606,13 @@
     <t>ORDER</t>
   </si>
   <si>
-    <t>FORUM</t>
+    <t>acknowledgedUsers</t>
+  </si>
+  <si>
+    <t>affectedUsers</t>
+  </si>
+  <si>
+    <t>relatedId</t>
   </si>
   <si>
     <t>priority</t>
@@ -612,19 +621,10 @@
     <t>eventTimestamp</t>
   </si>
   <si>
-    <t>affectedUsers</t>
-  </si>
-  <si>
-    <t>relatedId</t>
-  </si>
-  <si>
-    <t>acknowledgedUsers</t>
+    <t>id</t>
   </si>
   <si>
     <t>domain</t>
-  </si>
-  <si>
-    <t>id</t>
   </si>
   <si>
     <t>Source Class Name</t>
@@ -8712,7 +8712,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -8720,13 +8720,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4">
@@ -8734,13 +8734,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5">
@@ -8754,7 +8754,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -8762,13 +8762,13 @@
         <v>41</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7">
@@ -8776,13 +8776,13 @@
         <v>41</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8">
@@ -8894,7 +8894,7 @@
         <v>45</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16">
@@ -8908,7 +8908,7 @@
         <v>45</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17">
@@ -8922,7 +8922,7 @@
         <v>25</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
@@ -8930,13 +8930,13 @@
         <v>66</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19">
@@ -8944,13 +8944,13 @@
         <v>66</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
@@ -8964,7 +8964,7 @@
         <v>45</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21">
@@ -8978,7 +8978,7 @@
         <v>45</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22">
@@ -8992,7 +8992,7 @@
         <v>45</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
@@ -9020,7 +9020,7 @@
         <v>45</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25">
@@ -9034,7 +9034,7 @@
         <v>45</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26">
@@ -9048,7 +9048,7 @@
         <v>45</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>76</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -9076,7 +9076,7 @@
         <v>25</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
@@ -9084,13 +9084,13 @@
         <v>85</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30">
@@ -9098,13 +9098,13 @@
         <v>85</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31">
@@ -9112,7 +9112,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>45</v>
@@ -9126,7 +9126,7 @@
         <v>86</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>45</v>
@@ -9300,7 +9300,7 @@
         <v>45</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>76</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45">
@@ -9328,7 +9328,7 @@
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47">
@@ -9342,7 +9342,7 @@
         <v>25</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
@@ -9350,13 +9350,13 @@
         <v>104</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C48" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49">
@@ -9364,13 +9364,13 @@
         <v>104</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50">
@@ -9440,7 +9440,7 @@
         <v>25</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
@@ -9448,13 +9448,13 @@
         <v>108</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C55" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56">
@@ -9462,13 +9462,13 @@
         <v>108</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C56" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57">
@@ -9482,7 +9482,7 @@
         <v>45</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>42</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58">
@@ -9496,7 +9496,7 @@
         <v>45</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59">
@@ -9504,7 +9504,7 @@
         <v>109</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C59" t="s" s="0">
         <v>45</v>
@@ -9518,13 +9518,13 @@
         <v>109</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C60" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>123</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61">
@@ -9532,7 +9532,7 @@
         <v>109</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C61" t="s" s="0">
         <v>45</v>
@@ -9552,7 +9552,7 @@
         <v>45</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63">
@@ -9566,7 +9566,7 @@
         <v>45</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>105</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64">
@@ -9580,7 +9580,7 @@
         <v>45</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>13</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65">
@@ -9594,7 +9594,7 @@
         <v>25</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -9602,13 +9602,13 @@
         <v>118</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C66" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67">
@@ -9616,13 +9616,13 @@
         <v>118</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C67" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68">
@@ -9630,13 +9630,13 @@
         <v>111</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C68" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69">
@@ -9644,7 +9644,7 @@
         <v>111</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C69" t="s" s="0">
         <v>45</v>
@@ -9658,13 +9658,13 @@
         <v>111</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C70" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D70" t="s" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71">
@@ -9672,13 +9672,13 @@
         <v>111</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C71" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D71" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="72">
@@ -9686,13 +9686,13 @@
         <v>111</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="C72" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>105</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73">
@@ -9700,13 +9700,13 @@
         <v>111</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C73" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D73" t="s" s="0">
-        <v>123</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74">
@@ -9714,7 +9714,7 @@
         <v>111</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C74" t="s" s="0">
         <v>45</v>
@@ -9728,13 +9728,13 @@
         <v>111</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C75" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76">
@@ -9742,7 +9742,7 @@
         <v>87</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C76" t="s" s="0">
         <v>45</v>
@@ -9756,7 +9756,7 @@
         <v>87</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C77" t="s" s="0">
         <v>45</v>
@@ -9770,13 +9770,13 @@
         <v>62</v>
       </c>
       <c r="B78" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C78" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D78" t="s" s="0">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79">
@@ -9784,7 +9784,7 @@
         <v>62</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C79" t="s" s="0">
         <v>45</v>
@@ -9798,13 +9798,13 @@
         <v>62</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D80" t="s" s="0">
-        <v>127</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81">
@@ -9812,7 +9812,7 @@
         <v>95</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C81" t="s" s="0">
         <v>45</v>
@@ -9840,7 +9840,7 @@
         <v>95</v>
       </c>
       <c r="B83" t="s" s="0">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C83" t="s" s="0">
         <v>45</v>
@@ -9854,7 +9854,7 @@
         <v>95</v>
       </c>
       <c r="B84" t="s" s="0">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C84" t="s" s="0">
         <v>45</v>
@@ -9868,7 +9868,7 @@
         <v>95</v>
       </c>
       <c r="B85" t="s" s="0">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C85" t="s" s="0">
         <v>45</v>
@@ -9910,7 +9910,7 @@
         <v>95</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C88" t="s" s="0">
         <v>45</v>
@@ -9924,7 +9924,7 @@
         <v>95</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C89" t="s" s="0">
         <v>45</v>
@@ -9938,7 +9938,7 @@
         <v>95</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C90" t="s" s="0">
         <v>45</v>
@@ -9952,7 +9952,7 @@
         <v>95</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C91" t="s" s="0">
         <v>45</v>
@@ -9980,7 +9980,7 @@
         <v>70</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C93" t="s" s="0">
         <v>45</v>
@@ -9994,7 +9994,7 @@
         <v>70</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C94" t="s" s="0">
         <v>45</v>
@@ -10008,7 +10008,7 @@
         <v>70</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C95" t="s" s="0">
         <v>45</v>
@@ -10022,7 +10022,7 @@
         <v>70</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C96" t="s" s="0">
         <v>45</v>
@@ -10042,7 +10042,7 @@
         <v>25</v>
       </c>
       <c r="D97" t="s" s="0">
-        <v>161</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
@@ -10050,13 +10050,13 @@
         <v>153</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C98" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D98" t="s" s="0">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="99">
@@ -10064,13 +10064,13 @@
         <v>153</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C99" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed few problems with parser.
</commit_message>
<xml_diff>
--- a/data/backend/activity-client_structure.xlsx
+++ b/data/backend/activity-client_structure.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2801" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="273">
   <si>
     <t>Class Name</t>
   </si>
@@ -669,55 +669,178 @@
     <t>Number of Lines</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>180</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>NewsletterNotFoundException(java.lang.String)</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
+    <t>NewsletterNotFoundException()</t>
+  </si>
+  <si>
+    <t>UserNotFoundException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>UserNotFoundException()</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Priority(java.lang.String, int)</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
-    <t>11</t>
+    <t>NewsletterDTO$NewsletterDTOBuilder()</t>
+  </si>
+  <si>
+    <t>ActivityNotFoundException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>ActivityNotFoundException()</t>
+  </si>
+  <si>
+    <t>UserProfileDTO$UserProfileDTOBuilder()</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>ActivityQuerySpecification(java.lang.String, java.lang.Integer, java.lang.Integer)</t>
+  </si>
+  <si>
+    <t>ActivityQuerySpecification()</t>
+  </si>
+  <si>
+    <t>NewsletterException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>NewsletterException()</t>
+  </si>
+  <si>
+    <t>UserImageDTO$UserImageDTOBuilder()</t>
+  </si>
+  <si>
+    <t>UpdatedUserDetailsDTO$UpdatedUserDetailsDTOBuilder()</t>
+  </si>
+  <si>
+    <t>ActivityQuerySpecification$ActivityQuerySpecificationBuilder()</t>
+  </si>
+  <si>
+    <t>ActivityException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>ActivityException()</t>
+  </si>
+  <si>
+    <t>Domain(java.lang.String, int)</t>
+  </si>
+  <si>
+    <t>ActivityConflictException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>ActivityConflictException()</t>
+  </si>
+  <si>
+    <t>ActivityDTO$ActivityDTOBuilder()</t>
+  </si>
+  <si>
+    <t>NewsletterConflictException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>NewsletterConflictException()</t>
+  </si>
+  <si>
+    <t>ActivityDTO(java.lang.String, org.andante.activity.enums.Priority, org.andante.activity.enums.Domain, java.lang.String, java.util.Set, java.util.Set, java.lang.String, java.time.LocalDateTime)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>ActivityDTO()</t>
+  </si>
+  <si>
+    <t>UserImageDTO(java.lang.String, java.lang.String)</t>
+  </si>
+  <si>
+    <t>UserImageDTO()</t>
+  </si>
+  <si>
+    <t>NewsletterDTO(java.lang.String, java.time.LocalDateTime, java.lang.Boolean)</t>
+  </si>
+  <si>
+    <t>NewsletterDTO()</t>
+  </si>
+  <si>
+    <t>UpdatedUserDetailsDTO(java.lang.String, java.lang.String, java.lang.String, java.lang.String, java.lang.String, java.lang.String, java.lang.String, java.lang.String, java.lang.String, java.lang.String, java.lang.String)</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>UpdatedUserDetailsDTO()</t>
+  </si>
+  <si>
+    <t>75</t>
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>UserProfileDTO(java.lang.String, java.lang.String, java.lang.String, java.util.Set, java.util.Set)</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>UserConflictException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>UserConflictException()</t>
   </si>
 </sst>
 </file>
@@ -7364,7 +7487,7 @@
         <v>62</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21">
@@ -7372,7 +7495,7 @@
         <v>95</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22">
@@ -7380,7 +7503,7 @@
         <v>70</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23">
@@ -7398,7 +7521,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7417,46 +7540,46 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>50</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>206</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>43</v>
+        <v>231</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>48</v>
+        <v>232</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>12</v>
+        <v>233</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6">
@@ -7464,10 +7587,10 @@
         <v>42</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7">
@@ -7475,10 +7598,10 @@
         <v>42</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8">
@@ -7486,241 +7609,241 @@
         <v>42</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>206</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>61</v>
+        <v>237</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>12</v>
+        <v>238</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>82</v>
+        <v>239</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>84</v>
+        <v>240</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30">
@@ -7728,7 +7851,7 @@
         <v>74</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>230</v>
@@ -7739,912 +7862,1297 @@
         <v>74</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>90</v>
+        <v>242</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>97</v>
+        <v>243</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>229</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>99</v>
+        <v>244</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>94</v>
+        <v>245</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>229</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s" s="0">
         <v>61</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s" s="0">
         <v>12</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>101</v>
+        <v>246</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>229</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>206</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>206</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>206</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>116</v>
+        <v>247</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>229</v>
+        <v>207</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="C68" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>61</v>
+        <v>248</v>
       </c>
       <c r="C69" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>12</v>
+        <v>249</v>
       </c>
       <c r="C70" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>82</v>
+        <v>250</v>
       </c>
       <c r="C71" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>120</v>
+        <v>43</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>121</v>
+        <v>48</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="C75" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="0">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B78" t="s" s="0">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="0">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>126</v>
+        <v>251</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="0">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>82</v>
+        <v>252</v>
       </c>
       <c r="C80" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="0">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>129</v>
+        <v>253</v>
       </c>
       <c r="C81" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="0">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B82" t="s" s="0">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="0">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="B83" t="s" s="0">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s" s="0">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="B84" t="s" s="0">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s" s="0">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="B85" t="s" s="0">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s" s="0">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="B86" t="s" s="0">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B87" t="s" s="0">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="C91" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s" s="0">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>140</v>
+        <v>254</v>
       </c>
       <c r="C92" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s" s="0">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>137</v>
+        <v>255</v>
       </c>
       <c r="C93" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s" s="0">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>135</v>
+        <v>256</v>
       </c>
       <c r="C94" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="C95" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C96" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B97" t="s" s="0">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C97" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C98" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s" s="0">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="C99" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s" s="0">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B100" t="s" s="0">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="C100" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s" s="0">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B101" t="s" s="0">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C101" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s" s="0">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B102" t="s" s="0">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C102" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s" s="0">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B103" t="s" s="0">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="C103" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s" s="0">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>145</v>
+        <v>257</v>
       </c>
       <c r="C104" t="s" s="0">
-        <v>228</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s" s="0">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="B105" t="s" s="0">
-        <v>150</v>
+        <v>259</v>
       </c>
       <c r="C105" t="s" s="0">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s" s="0">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B106" t="s" s="0">
-        <v>148</v>
+        <v>82</v>
       </c>
       <c r="C106" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s" s="0">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s" s="0">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="C107" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s" s="0">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B108" t="s" s="0">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C108" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s" s="0">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B109" t="s" s="0">
-        <v>147</v>
+        <v>260</v>
       </c>
       <c r="C109" t="s" s="0">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s" s="0">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B110" t="s" s="0">
-        <v>5</v>
+        <v>261</v>
       </c>
       <c r="C110" t="s" s="0">
-        <v>229</v>
+        <v>207</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B111" t="s" s="0">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C111" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s" s="0">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B112" t="s" s="0">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="C112" t="s" s="0">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B113" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="C113" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B114" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="C114" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B115" t="s" s="0">
+        <v>262</v>
+      </c>
+      <c r="C115" t="s" s="0">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B116" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="C116" t="s" s="0">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B117" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C117" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B118" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="C118" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B119" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="C119" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B120" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="C120" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B121" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="C121" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B122" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="C122" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B123" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="C123" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B124" t="s" s="0">
+        <v>135</v>
+      </c>
+      <c r="C124" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B125" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="C125" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B126" t="s" s="0">
+        <v>143</v>
+      </c>
+      <c r="C126" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B127" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="C127" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B128" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="C128" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B129" t="s" s="0">
+        <v>264</v>
+      </c>
+      <c r="C129" t="s" s="0">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B130" t="s" s="0">
+        <v>266</v>
+      </c>
+      <c r="C130" t="s" s="0">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="B113" t="s" s="0">
+      <c r="B131" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="C131" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B132" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="C132" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B133" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="C133" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B134" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="C134" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B135" t="s" s="0">
+        <v>151</v>
+      </c>
+      <c r="C135" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B136" t="s" s="0">
+        <v>145</v>
+      </c>
+      <c r="C136" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B137" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="C137" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B138" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="C138" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B139" t="s" s="0">
+        <v>149</v>
+      </c>
+      <c r="C139" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B140" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="C140" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B141" t="s" s="0">
+        <v>147</v>
+      </c>
+      <c r="C141" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B142" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C142" t="s" s="0">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B143" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="C143" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B144" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C144" t="s" s="0">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B145" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="C113" t="s" s="0">
-        <v>228</v>
+      <c r="C145" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B146" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="C146" t="s" s="0">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="B147" t="s" s="0">
+        <v>271</v>
+      </c>
+      <c r="C147" t="s" s="0">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="0">
+        <v>153</v>
+      </c>
+      <c r="B148" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="C148" t="s" s="0">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored Parser structure. Fixed problems with reading size od classes and methods.
</commit_message>
<xml_diff>
--- a/data/backend/activity-client_structure.xlsx
+++ b/data/backend/activity-client_structure.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="272">
   <si>
     <t>Class Name</t>
   </si>
@@ -504,129 +504,129 @@
     <t>Field Type</t>
   </si>
   <si>
+    <t>serialVersionUID</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
     <t>$assertionsDisabled</t>
   </si>
   <si>
-    <t>serialVersionUID</t>
-  </si>
-  <si>
-    <t>long</t>
+    <t>HIGHEST</t>
+  </si>
+  <si>
+    <t>HIGH</t>
   </si>
   <si>
     <t>LOW</t>
   </si>
   <si>
+    <t>$VALUES</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
     <t>LOWEST</t>
   </si>
   <si>
-    <t>HIGH</t>
-  </si>
-  <si>
-    <t>HIGHEST</t>
-  </si>
-  <si>
-    <t>$VALUES</t>
-  </si>
-  <si>
-    <t>MEDIUM</t>
+    <t>isConfirmed</t>
   </si>
   <si>
     <t>emailAddress</t>
   </si>
   <si>
-    <t>isConfirmed</t>
-  </si>
-  <si>
     <t>subscriptionDate</t>
   </si>
   <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>imageUrl</t>
+  </si>
+  <si>
     <t>observedUsers</t>
   </si>
   <si>
     <t>observingUsers</t>
   </si>
   <si>
-    <t>imageUrl</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>username</t>
+    <t>query</t>
   </si>
   <si>
     <t>pageSize</t>
   </si>
   <si>
-    <t>query</t>
-  </si>
-  <si>
     <t>pageNumber</t>
   </si>
   <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
     <t>phoneNumber</t>
   </si>
   <si>
-    <t>street</t>
+    <t>city</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
   <si>
     <t>profileImageUrl</t>
   </si>
   <si>
-    <t>dateOfBirth</t>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>country</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>postalCode</t>
-  </si>
-  <si>
     <t>FORUM</t>
   </si>
   <si>
+    <t>ORDER</t>
+  </si>
+  <si>
     <t>PRODUCT</t>
   </si>
   <si>
-    <t>ORDER</t>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>relatedId</t>
+  </si>
+  <si>
+    <t>affectedUsers</t>
   </si>
   <si>
     <t>acknowledgedUsers</t>
   </si>
   <si>
-    <t>affectedUsers</t>
-  </si>
-  <si>
-    <t>relatedId</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
     <t>eventTimestamp</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
     <t>Source Class Name</t>
   </si>
   <si>
@@ -669,90 +669,93 @@
     <t>Number of Lines</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>NewsletterNotFoundException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>NewsletterNotFoundException()</t>
+  </si>
+  <si>
+    <t>UserNotFoundException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>UserNotFoundException()</t>
+  </si>
+  <si>
+    <t>Priority(java.lang.String, int)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>NewsletterDTO$NewsletterDTOBuilder()</t>
+  </si>
+  <si>
+    <t>ActivityNotFoundException(java.lang.String)</t>
+  </si>
+  <si>
+    <t>ActivityNotFoundException()</t>
+  </si>
+  <si>
+    <t>UserProfileDTO$UserProfileDTOBuilder()</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>ActivityQuerySpecification(java.lang.String, java.lang.Integer, java.lang.Integer)</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>NewsletterNotFoundException(java.lang.String)</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>NewsletterNotFoundException()</t>
-  </si>
-  <si>
-    <t>UserNotFoundException(java.lang.String)</t>
-  </si>
-  <si>
-    <t>UserNotFoundException()</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Priority(java.lang.String, int)</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>NewsletterDTO$NewsletterDTOBuilder()</t>
-  </si>
-  <si>
-    <t>ActivityNotFoundException(java.lang.String)</t>
-  </si>
-  <si>
-    <t>ActivityNotFoundException()</t>
-  </si>
-  <si>
-    <t>UserProfileDTO$UserProfileDTOBuilder()</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>ActivityQuerySpecification(java.lang.String, java.lang.Integer, java.lang.Integer)</t>
-  </si>
-  <si>
     <t>ActivityQuerySpecification()</t>
   </si>
   <si>
@@ -798,9 +801,6 @@
     <t>ActivityDTO(java.lang.String, org.andante.activity.enums.Priority, org.andante.activity.enums.Domain, java.lang.String, java.util.Set, java.util.Set, java.lang.String, java.time.LocalDateTime)</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>ActivityDTO()</t>
   </si>
   <si>
@@ -832,9 +832,6 @@
   </si>
   <si>
     <t>UserProfileDTO(java.lang.String, java.lang.String, java.lang.String, java.util.Set, java.util.Set)</t>
-  </si>
-  <si>
-    <t>7</t>
   </si>
   <si>
     <t>UserConflictException(java.lang.String)</t>
@@ -7590,7 +7587,7 @@
         <v>50</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7">
@@ -7601,7 +7598,7 @@
         <v>43</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8">
@@ -7634,7 +7631,7 @@
         <v>58</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11">
@@ -7645,7 +7642,7 @@
         <v>44</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12">
@@ -7656,7 +7653,7 @@
         <v>56</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13">
@@ -7664,10 +7661,10 @@
         <v>42</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14">
@@ -7678,7 +7675,7 @@
         <v>64</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15">
@@ -7689,7 +7686,7 @@
         <v>65</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16">
@@ -7700,7 +7697,7 @@
         <v>63</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17">
@@ -7730,7 +7727,7 @@
         <v>60</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>207</v>
@@ -7741,7 +7738,7 @@
         <v>66</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>230</v>
@@ -7752,7 +7749,7 @@
         <v>66</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>207</v>
@@ -7766,7 +7763,7 @@
         <v>68</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23">
@@ -7777,7 +7774,7 @@
         <v>71</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24">
@@ -7788,7 +7785,7 @@
         <v>72</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25">
@@ -7799,7 +7796,7 @@
         <v>69</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26">
@@ -7810,7 +7807,7 @@
         <v>73</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27">
@@ -7840,7 +7837,7 @@
         <v>67</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>207</v>
@@ -7931,7 +7928,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38">
@@ -7953,7 +7950,7 @@
         <v>20</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>216</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40">
@@ -7975,7 +7972,7 @@
         <v>242</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>215</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42">
@@ -7983,7 +7980,7 @@
         <v>74</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C42" t="s" s="0">
         <v>207</v>
@@ -7994,7 +7991,7 @@
         <v>85</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C43" t="s" s="0">
         <v>230</v>
@@ -8005,7 +8002,7 @@
         <v>85</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C44" t="s" s="0">
         <v>207</v>
@@ -8019,7 +8016,7 @@
         <v>71</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46">
@@ -8030,7 +8027,7 @@
         <v>72</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47">
@@ -8060,7 +8057,7 @@
         <v>86</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>207</v>
@@ -8074,7 +8071,7 @@
         <v>96</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51">
@@ -8085,7 +8082,7 @@
         <v>98</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52">
@@ -8096,7 +8093,7 @@
         <v>91</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53">
@@ -8107,7 +8104,7 @@
         <v>93</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54">
@@ -8118,7 +8115,7 @@
         <v>100</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55">
@@ -8129,7 +8126,7 @@
         <v>90</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56">
@@ -8140,7 +8137,7 @@
         <v>97</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57">
@@ -8151,7 +8148,7 @@
         <v>99</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58">
@@ -8162,7 +8159,7 @@
         <v>94</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59">
@@ -8173,7 +8170,7 @@
         <v>92</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60">
@@ -8184,7 +8181,7 @@
         <v>89</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61">
@@ -8214,7 +8211,7 @@
         <v>88</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C63" t="s" s="0">
         <v>207</v>
@@ -8228,7 +8225,7 @@
         <v>101</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65">
@@ -8239,7 +8236,7 @@
         <v>103</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="66">
@@ -8250,7 +8247,7 @@
         <v>102</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67">
@@ -8280,7 +8277,7 @@
         <v>83</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C69" t="s" s="0">
         <v>207</v>
@@ -8291,7 +8288,7 @@
         <v>104</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C70" t="s" s="0">
         <v>230</v>
@@ -8302,7 +8299,7 @@
         <v>104</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C71" t="s" s="0">
         <v>207</v>
@@ -8316,7 +8313,7 @@
         <v>50</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73">
@@ -8327,7 +8324,7 @@
         <v>43</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74">
@@ -8360,7 +8357,7 @@
         <v>58</v>
       </c>
       <c r="C76" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="77">
@@ -8371,7 +8368,7 @@
         <v>106</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="78">
@@ -8382,7 +8379,7 @@
         <v>56</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="79">
@@ -8390,10 +8387,10 @@
         <v>105</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80">
@@ -8401,7 +8398,7 @@
         <v>108</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C80" t="s" s="0">
         <v>230</v>
@@ -8412,7 +8409,7 @@
         <v>108</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C81" t="s" s="0">
         <v>207</v>
@@ -8426,7 +8423,7 @@
         <v>112</v>
       </c>
       <c r="C82" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83">
@@ -8437,7 +8434,7 @@
         <v>110</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="84">
@@ -8448,7 +8445,7 @@
         <v>116</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85">
@@ -8459,7 +8456,7 @@
         <v>114</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="86">
@@ -8470,7 +8467,7 @@
         <v>117</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="87">
@@ -8481,7 +8478,7 @@
         <v>115</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="88">
@@ -8492,7 +8489,7 @@
         <v>89</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="89">
@@ -8503,7 +8500,7 @@
         <v>113</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="90">
@@ -8533,7 +8530,7 @@
         <v>109</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C92" t="s" s="0">
         <v>207</v>
@@ -8544,7 +8541,7 @@
         <v>118</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C93" t="s" s="0">
         <v>230</v>
@@ -8555,7 +8552,7 @@
         <v>118</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C94" t="s" s="0">
         <v>207</v>
@@ -8665,10 +8662,10 @@
         <v>111</v>
       </c>
       <c r="B104" t="s" s="0">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C104" t="s" s="0">
-        <v>258</v>
+        <v>222</v>
       </c>
     </row>
     <row r="105">
@@ -8723,7 +8720,7 @@
         <v>260</v>
       </c>
       <c r="C109" t="s" s="0">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="110">
@@ -8789,7 +8786,7 @@
         <v>262</v>
       </c>
       <c r="C115" t="s" s="0">
-        <v>215</v>
+        <v>243</v>
       </c>
     </row>
     <row r="116">
@@ -9130,7 +9127,7 @@
         <v>269</v>
       </c>
       <c r="C146" t="s" s="0">
-        <v>270</v>
+        <v>215</v>
       </c>
     </row>
     <row r="147">
@@ -9138,7 +9135,7 @@
         <v>153</v>
       </c>
       <c r="B147" t="s" s="0">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C147" t="s" s="0">
         <v>230</v>
@@ -9149,7 +9146,7 @@
         <v>153</v>
       </c>
       <c r="B148" t="s" s="0">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C148" t="s" s="0">
         <v>207</v>
@@ -9220,7 +9217,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3">
@@ -9228,13 +9225,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4">
@@ -9242,13 +9239,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -9262,7 +9259,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6">
@@ -9270,13 +9267,13 @@
         <v>41</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7">
@@ -9284,13 +9281,13 @@
         <v>41</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -9343,10 +9340,10 @@
         <v>166</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
@@ -9357,10 +9354,10 @@
         <v>167</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
@@ -9388,7 +9385,7 @@
         <v>45</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>13</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15">
@@ -9402,7 +9399,7 @@
         <v>45</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>133</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -9430,7 +9427,7 @@
         <v>25</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
@@ -9438,13 +9435,13 @@
         <v>66</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19">
@@ -9452,13 +9449,13 @@
         <v>66</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
@@ -9472,7 +9469,7 @@
         <v>45</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -9486,7 +9483,7 @@
         <v>45</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22">
@@ -9514,7 +9511,7 @@
         <v>45</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24">
@@ -9528,7 +9525,7 @@
         <v>45</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25">
@@ -9542,7 +9539,7 @@
         <v>45</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>76</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26">
@@ -9556,7 +9553,7 @@
         <v>45</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27">
@@ -9584,7 +9581,7 @@
         <v>25</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29">
@@ -9592,13 +9589,13 @@
         <v>85</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30">
@@ -9606,13 +9603,13 @@
         <v>85</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
@@ -9620,7 +9617,7 @@
         <v>86</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>45</v>
@@ -9634,7 +9631,7 @@
         <v>86</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>45</v>
@@ -9808,7 +9805,7 @@
         <v>45</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45">
@@ -9816,13 +9813,13 @@
         <v>83</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C45" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>76</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
@@ -9830,7 +9827,7 @@
         <v>83</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>45</v>
@@ -9850,7 +9847,7 @@
         <v>25</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48">
@@ -9858,13 +9855,13 @@
         <v>104</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49">
@@ -9872,13 +9869,13 @@
         <v>104</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
@@ -9914,7 +9911,7 @@
         <v>105</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s" s="0">
         <v>45</v>
@@ -9948,7 +9945,7 @@
         <v>25</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55">
@@ -9956,13 +9953,13 @@
         <v>108</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C55" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56">
@@ -9970,13 +9967,13 @@
         <v>108</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C56" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
@@ -9990,7 +9987,7 @@
         <v>45</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58">
@@ -10004,7 +10001,7 @@
         <v>45</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>123</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59">
@@ -10032,7 +10029,7 @@
         <v>45</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61">
@@ -10040,13 +10037,13 @@
         <v>109</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="C61" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62">
@@ -10054,13 +10051,13 @@
         <v>109</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C62" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>127</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63">
@@ -10074,7 +10071,7 @@
         <v>45</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64">
@@ -10088,7 +10085,7 @@
         <v>45</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65">
@@ -10102,7 +10099,7 @@
         <v>25</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66">
@@ -10110,13 +10107,13 @@
         <v>118</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C66" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67">
@@ -10124,13 +10121,13 @@
         <v>118</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C67" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
@@ -10144,7 +10141,7 @@
         <v>45</v>
       </c>
       <c r="D68" t="s" s="0">
-        <v>123</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69">
@@ -10158,7 +10155,7 @@
         <v>45</v>
       </c>
       <c r="D69" t="s" s="0">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70">
@@ -10180,13 +10177,13 @@
         <v>111</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C71" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D71" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72">
@@ -10194,13 +10191,13 @@
         <v>111</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C72" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D72" t="s" s="0">
-        <v>13</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73">
@@ -10214,7 +10211,7 @@
         <v>45</v>
       </c>
       <c r="D73" t="s" s="0">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74">
@@ -10228,7 +10225,7 @@
         <v>45</v>
       </c>
       <c r="D74" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75">
@@ -10242,7 +10239,7 @@
         <v>45</v>
       </c>
       <c r="D75" t="s" s="0">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76">
@@ -10250,7 +10247,7 @@
         <v>87</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C76" t="s" s="0">
         <v>45</v>
@@ -10264,7 +10261,7 @@
         <v>87</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C77" t="s" s="0">
         <v>45</v>
@@ -10292,7 +10289,7 @@
         <v>62</v>
       </c>
       <c r="B79" t="s" s="0">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C79" t="s" s="0">
         <v>45</v>
@@ -10306,7 +10303,7 @@
         <v>62</v>
       </c>
       <c r="B80" t="s" s="0">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C80" t="s" s="0">
         <v>45</v>
@@ -10320,7 +10317,7 @@
         <v>95</v>
       </c>
       <c r="B81" t="s" s="0">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C81" t="s" s="0">
         <v>45</v>
@@ -10334,7 +10331,7 @@
         <v>95</v>
       </c>
       <c r="B82" t="s" s="0">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C82" t="s" s="0">
         <v>45</v>
@@ -10348,7 +10345,7 @@
         <v>95</v>
       </c>
       <c r="B83" t="s" s="0">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C83" t="s" s="0">
         <v>45</v>
@@ -10362,7 +10359,7 @@
         <v>95</v>
       </c>
       <c r="B84" t="s" s="0">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C84" t="s" s="0">
         <v>45</v>
@@ -10376,7 +10373,7 @@
         <v>95</v>
       </c>
       <c r="B85" t="s" s="0">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C85" t="s" s="0">
         <v>45</v>
@@ -10390,7 +10387,7 @@
         <v>95</v>
       </c>
       <c r="B86" t="s" s="0">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C86" t="s" s="0">
         <v>45</v>
@@ -10404,7 +10401,7 @@
         <v>95</v>
       </c>
       <c r="B87" t="s" s="0">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C87" t="s" s="0">
         <v>45</v>
@@ -10418,7 +10415,7 @@
         <v>95</v>
       </c>
       <c r="B88" t="s" s="0">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C88" t="s" s="0">
         <v>45</v>
@@ -10432,7 +10429,7 @@
         <v>95</v>
       </c>
       <c r="B89" t="s" s="0">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C89" t="s" s="0">
         <v>45</v>
@@ -10446,7 +10443,7 @@
         <v>95</v>
       </c>
       <c r="B90" t="s" s="0">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C90" t="s" s="0">
         <v>45</v>
@@ -10460,7 +10457,7 @@
         <v>95</v>
       </c>
       <c r="B91" t="s" s="0">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C91" t="s" s="0">
         <v>45</v>
@@ -10474,7 +10471,7 @@
         <v>70</v>
       </c>
       <c r="B92" t="s" s="0">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C92" t="s" s="0">
         <v>45</v>
@@ -10488,13 +10485,13 @@
         <v>70</v>
       </c>
       <c r="B93" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C93" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D93" t="s" s="0">
-        <v>123</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94">
@@ -10502,7 +10499,7 @@
         <v>70</v>
       </c>
       <c r="B94" t="s" s="0">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C94" t="s" s="0">
         <v>45</v>
@@ -10516,7 +10513,7 @@
         <v>70</v>
       </c>
       <c r="B95" t="s" s="0">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C95" t="s" s="0">
         <v>45</v>
@@ -10530,13 +10527,13 @@
         <v>70</v>
       </c>
       <c r="B96" t="s" s="0">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C96" t="s" s="0">
         <v>45</v>
       </c>
       <c r="D96" t="s" s="0">
-        <v>13</v>
+        <v>123</v>
       </c>
     </row>
     <row r="97">
@@ -10550,7 +10547,7 @@
         <v>25</v>
       </c>
       <c r="D97" t="s" s="0">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98">
@@ -10558,13 +10555,13 @@
         <v>153</v>
       </c>
       <c r="B98" t="s" s="0">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C98" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D98" t="s" s="0">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99">
@@ -10572,13 +10569,13 @@
         <v>153</v>
       </c>
       <c r="B99" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C99" t="s" s="0">
         <v>25</v>
       </c>
       <c r="D99" t="s" s="0">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed errors with MSM implementation.
</commit_message>
<xml_diff>
--- a/data/backend/activity-client_structure.xlsx
+++ b/data/backend/activity-client_structure.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="273">
   <si>
     <t>Class Name</t>
   </si>
@@ -817,6 +817,9 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>4</t>
@@ -8077,7 +8080,7 @@
         <v>53</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7">
@@ -8088,7 +8091,7 @@
         <v>47</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8">
@@ -8099,7 +8102,7 @@
         <v>50</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9">
@@ -8132,7 +8135,7 @@
         <v>57</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12">
@@ -8143,7 +8146,7 @@
         <v>48</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13">
@@ -8154,7 +8157,7 @@
         <v>55</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14">
@@ -8176,7 +8179,7 @@
         <v>70</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16">
@@ -8187,7 +8190,7 @@
         <v>71</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17">
@@ -8198,7 +8201,7 @@
         <v>69</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18">
@@ -8264,7 +8267,7 @@
         <v>76</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24">
@@ -8275,7 +8278,7 @@
         <v>80</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25">
@@ -8286,7 +8289,7 @@
         <v>81</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26">
@@ -8297,7 +8300,7 @@
         <v>77</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27">
@@ -8308,7 +8311,7 @@
         <v>82</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28">
@@ -8418,7 +8421,7 @@
         <v>5</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38">
@@ -8440,7 +8443,7 @@
         <v>15</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40">
@@ -8462,7 +8465,7 @@
         <v>84</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42">
@@ -8517,7 +8520,7 @@
         <v>80</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47">
@@ -8528,7 +8531,7 @@
         <v>81</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48">
@@ -8572,7 +8575,7 @@
         <v>110</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52">
@@ -8583,7 +8586,7 @@
         <v>112</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53">
@@ -8594,7 +8597,7 @@
         <v>105</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54">
@@ -8605,7 +8608,7 @@
         <v>107</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55">
@@ -8616,7 +8619,7 @@
         <v>114</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56">
@@ -8627,7 +8630,7 @@
         <v>104</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57">
@@ -8638,7 +8641,7 @@
         <v>111</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58">
@@ -8649,7 +8652,7 @@
         <v>113</v>
       </c>
       <c r="C58" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59">
@@ -8660,7 +8663,7 @@
         <v>108</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60">
@@ -8671,7 +8674,7 @@
         <v>106</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61">
@@ -8682,7 +8685,7 @@
         <v>103</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="62">
@@ -8726,7 +8729,7 @@
         <v>116</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="66">
@@ -8737,7 +8740,7 @@
         <v>119</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67">
@@ -8748,7 +8751,7 @@
         <v>117</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68">
@@ -8803,7 +8806,7 @@
         <v>53</v>
       </c>
       <c r="C72" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73">
@@ -8814,7 +8817,7 @@
         <v>47</v>
       </c>
       <c r="C73" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74">
@@ -8825,7 +8828,7 @@
         <v>124</v>
       </c>
       <c r="C74" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75">
@@ -8858,7 +8861,7 @@
         <v>57</v>
       </c>
       <c r="C77" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78">
@@ -8869,7 +8872,7 @@
         <v>125</v>
       </c>
       <c r="C78" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79">
@@ -8880,7 +8883,7 @@
         <v>55</v>
       </c>
       <c r="C79" t="s" s="0">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="80">
@@ -8924,7 +8927,7 @@
         <v>134</v>
       </c>
       <c r="C83" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="84">
@@ -8935,7 +8938,7 @@
         <v>131</v>
       </c>
       <c r="C84" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="85">
@@ -8946,7 +8949,7 @@
         <v>138</v>
       </c>
       <c r="C85" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="86">
@@ -8957,7 +8960,7 @@
         <v>136</v>
       </c>
       <c r="C86" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="87">
@@ -8968,7 +8971,7 @@
         <v>139</v>
       </c>
       <c r="C87" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="88">
@@ -8979,7 +8982,7 @@
         <v>137</v>
       </c>
       <c r="C88" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89">
@@ -8990,7 +8993,7 @@
         <v>103</v>
       </c>
       <c r="C89" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90">
@@ -9001,7 +9004,7 @@
         <v>135</v>
       </c>
       <c r="C90" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="91">
@@ -9210,7 +9213,7 @@
         <v>157</v>
       </c>
       <c r="C109" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="110">
@@ -9276,7 +9279,7 @@
         <v>162</v>
       </c>
       <c r="C115" t="s" s="0">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="116">
@@ -9430,7 +9433,7 @@
         <v>174</v>
       </c>
       <c r="C129" t="s" s="0">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="130">
@@ -9584,7 +9587,7 @@
         <v>5</v>
       </c>
       <c r="C143" t="s" s="0">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="144">
@@ -9606,7 +9609,7 @@
         <v>15</v>
       </c>
       <c r="C145" t="s" s="0">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="146">

</xml_diff>